<commit_message>
Add python data prep code and save image as png
</commit_message>
<xml_diff>
--- a/Using Python in SAS Studio in SAS Viya/Excel Report with SAS Python and SQL/myExcelReport.xlsx
+++ b/Using Python in SAS Studio in SAS Viya/Excel Report with SAS Python and SQL/myExcelReport.xlsx
@@ -1667,27 +1667,18 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>73024</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" title="Graphics text slide" descr="Graphics text slide"/>
+        <xdr:cNvPr id="2" name="Picture 1" title="Data NULL Table"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId1"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19463,7 +19454,7 @@
   <sheetPr filterMode="0" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
     </sheetView>
@@ -19474,79 +19465,78 @@
     <col min="2" max="2" width="14.71" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="40" ht="12" customHeight="1"/>
-    <row r="41" ht="33" customHeight="1">
-      <c r="A41" s="8" t="s">
+    <row r="37" ht="33" customHeight="1">
+      <c r="A37" s="8" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="42" ht="12" customHeight="1"/>
-    <row r="43" ht="14" customHeight="1">
-      <c r="A43" s="9" t="s">
+    <row r="38" ht="12" customHeight="1"/>
+    <row r="39" ht="14" customHeight="1">
+      <c r="A39" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B39" s="10" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="44" ht="14" customHeight="1">
-      <c r="A44" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B44" s="11">
+    <row r="40" ht="14" customHeight="1">
+      <c r="A40" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="11">
         <v>25</v>
       </c>
     </row>
+    <row r="41" ht="14" customHeight="1">
+      <c r="A41" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="11">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" ht="14" customHeight="1">
+      <c r="A42" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" ht="12" customHeight="1"/>
+    <row r="44" ht="23" customHeight="1">
+      <c r="A44" s="12" t="s">
+        <v>492</v>
+      </c>
+    </row>
     <row r="45" ht="14" customHeight="1">
-      <c r="A45" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B45" s="11">
-        <v>23</v>
+      <c r="A45" s="0" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="46" ht="14" customHeight="1">
-      <c r="A46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B46" s="11">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="47" ht="12" customHeight="1"/>
-    <row r="48" ht="23" customHeight="1">
-      <c r="A48" s="12" t="s">
-        <v>492</v>
+      <c r="A46" s="13" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="47" ht="14" customHeight="1">
+      <c r="A47" s="13" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="48" ht="14" customHeight="1">
+      <c r="A48" s="13" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="49" ht="14" customHeight="1">
       <c r="A49" s="0" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="50" ht="14" customHeight="1">
-      <c r="A50" s="13" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="51" ht="14" customHeight="1">
-      <c r="A51" s="13" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="52" ht="14" customHeight="1">
-      <c r="A52" s="13" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="53" ht="14" customHeight="1">
-      <c r="A53" s="0" t="s">
         <v>497</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A41:J41"/>
+    <mergeCell ref="A37:J37"/>
   </mergeCells>
   <printOptions headings="0" horizontalCentered="0" verticalCentered="0" gridLines="0"/>
   <pageMargins left="0.05" right="0.05" top="0.5" bottom="0.5" header="0" footer="0"/>

</xml_diff>